<commit_message>
Ajout taux d'emploi au total par trimestre
</commit_message>
<xml_diff>
--- a/Table/taux d'emploi par trim et nature employeur.xlsx
+++ b/Table/taux d'emploi par trim et nature employeur.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serine/Desktop/Cours 3A/Projet DSSS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serine/Bureau/GitHub/PDSSS/Table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB460DFC-FB59-E242-94E8-D3B054E9A4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E82FA6-082F-A44C-8AC7-3E3D27952D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{7F62AEF7-FE98-2740-A318-B2317C90E55A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>Nature de l'employeur</t>
   </si>
@@ -204,13 +204,50 @@
   </si>
   <si>
     <t>59.2%</t>
+  </si>
+  <si>
+    <t>% en emploi</t>
+  </si>
+  <si>
+    <t>46.4 %</t>
+  </si>
+  <si>
+    <t>46.3%</t>
+  </si>
+  <si>
+    <t>46.2%</t>
+  </si>
+  <si>
+    <t>46.5%</t>
+  </si>
+  <si>
+    <t>46.1%</t>
+  </si>
+  <si>
+    <t>46.6%</t>
+  </si>
+  <si>
+    <t>46.7%</t>
+  </si>
+  <si>
+    <t>45.7%</t>
+  </si>
+  <si>
+    <t>46.4%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,12 +256,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -236,15 +279,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -556,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2172810-C190-B54D-B4AC-A5385D3A3377}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,6 +935,47 @@
         <v>41</v>
       </c>
     </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>